<commit_message>
Documentation Changes updates for Arduino
</commit_message>
<xml_diff>
--- a/documentation/microturbineManifast20160930.xlsx
+++ b/documentation/microturbineManifast20160930.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -100,9 +100,6 @@
     <t>18Amp 2-4S LiPo ESC</t>
   </si>
   <si>
-    <t>LXFTVP</t>
-  </si>
-  <si>
     <t>http://www3.towerhobbies.com/cgi-bin/wti0001p?&amp;I=LXFTVP&amp;P=7</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>EEA-GA1E100</t>
   </si>
   <si>
-    <t>Cap 10 uF, 25 VDC</t>
-  </si>
-  <si>
     <t>http://www.mouser.com/Search/Refine.aspx?Keyword=EEA-GA1E100</t>
   </si>
   <si>
@@ -254,6 +248,21 @@
   </si>
   <si>
     <t>HST-187B</t>
+  </si>
+  <si>
+    <t>LXFTVP Energy Rotor</t>
+  </si>
+  <si>
+    <t>T322A105J020AS</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/Search/ProductDetail.aspx?R=T322A105J020ASvirtualkey64600000virtualkey80-T322A105J020</t>
+  </si>
+  <si>
+    <t>Cap 1 uF, 20 VDC, 5%</t>
+  </si>
+  <si>
+    <t>Cap 10 uF, 25 VDC, 20%</t>
   </si>
 </sst>
 </file>
@@ -452,7 +461,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -484,6 +493,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -790,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,8 +844,8 @@
         <v>9</v>
       </c>
       <c r="I1" s="12">
-        <f>SUM(I2:I21)</f>
-        <v>185.82584</v>
+        <f>SUM(I2:I22)</f>
+        <v>186.72344000000001</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -856,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="6">
-        <f>E2*F2</f>
+        <f t="shared" ref="G2:G9" si="0">E2*F2</f>
         <v>40.520000000000003</v>
       </c>
       <c r="H2" s="6">
@@ -874,11 +886,11 @@
       <c r="B3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="E3" s="6">
         <v>19.989999999999998</v>
@@ -887,14 +899,14 @@
         <v>1</v>
       </c>
       <c r="G3" s="6">
-        <f>E3*F3</f>
+        <f t="shared" si="0"/>
         <v>19.989999999999998</v>
       </c>
       <c r="H3" s="6">
         <v>3.99</v>
       </c>
       <c r="I3" s="15">
-        <f>G3+H3</f>
+        <f t="shared" ref="I3:I9" si="1">G3+H3</f>
         <v>23.979999999999997</v>
       </c>
     </row>
@@ -918,14 +930,14 @@
         <v>1</v>
       </c>
       <c r="G4" s="6">
-        <f>E4*F4</f>
+        <f t="shared" si="0"/>
         <v>18.59</v>
       </c>
       <c r="H4" s="8">
         <v>0</v>
       </c>
       <c r="I4" s="15">
-        <f>G4+H4</f>
+        <f t="shared" si="1"/>
         <v>18.59</v>
       </c>
     </row>
@@ -947,14 +959,14 @@
         <v>1</v>
       </c>
       <c r="G5" s="6">
-        <f>E5*F5</f>
+        <f t="shared" si="0"/>
         <v>17.989999999999998</v>
       </c>
       <c r="H5" s="8">
         <v>0</v>
       </c>
       <c r="I5" s="15">
-        <f>G5+H5</f>
+        <f t="shared" si="1"/>
         <v>17.989999999999998</v>
       </c>
     </row>
@@ -978,29 +990,29 @@
         <v>1</v>
       </c>
       <c r="G6" s="6">
-        <f>E6*F6</f>
+        <f t="shared" si="0"/>
         <v>16.86</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
       </c>
       <c r="I6" s="15">
-        <f>G6+H6</f>
+        <f t="shared" si="1"/>
         <v>16.86</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="6">
         <v>4.99</v>
@@ -1009,7 +1021,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="6">
-        <f>E7*F7</f>
+        <f t="shared" si="0"/>
         <v>9.98</v>
       </c>
       <c r="H7" s="8">
@@ -1017,22 +1029,22 @@
         <v>0.55888000000000004</v>
       </c>
       <c r="I7" s="15">
-        <f>G7+H7</f>
+        <f t="shared" si="1"/>
         <v>10.538880000000001</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>65</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="6">
         <v>9.9700000000000006</v>
@@ -1041,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="6">
-        <f>E8*F8</f>
+        <f t="shared" si="0"/>
         <v>9.9700000000000006</v>
       </c>
       <c r="H8" s="8">
@@ -1049,22 +1061,22 @@
         <v>0.55832000000000004</v>
       </c>
       <c r="I8" s="15">
-        <f>G8+H8</f>
+        <f t="shared" si="1"/>
         <v>10.528320000000001</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="4">
         <v>17331512</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E9" s="6">
         <v>8.9700000000000006</v>
@@ -1073,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="6">
-        <f>E9*F9</f>
+        <f t="shared" si="0"/>
         <v>8.9700000000000006</v>
       </c>
       <c r="H9" s="8">
@@ -1081,22 +1093,22 @@
         <v>0.5023200000000001</v>
       </c>
       <c r="I9" s="15">
-        <f>G9+H9</f>
+        <f t="shared" si="1"/>
         <v>9.4723199999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="6">
         <v>0</v>
@@ -1132,29 +1144,29 @@
         <v>1</v>
       </c>
       <c r="G11" s="6">
-        <f>E11*F11</f>
+        <f t="shared" ref="G11:G20" si="2">E11*F11</f>
         <v>6.89</v>
       </c>
       <c r="H11" s="8">
         <v>0</v>
       </c>
       <c r="I11" s="15">
-        <f>G11+H11</f>
+        <f t="shared" ref="I11:I20" si="3">G11+H11</f>
         <v>6.89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>62</v>
       </c>
       <c r="C12" s="4">
         <v>531137</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="6">
         <v>6.38</v>
@@ -1163,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="6">
-        <f>E12*F12</f>
+        <f t="shared" si="2"/>
         <v>6.38</v>
       </c>
       <c r="H12" s="8">
@@ -1171,22 +1183,22 @@
         <v>0.35727999999999999</v>
       </c>
       <c r="I12" s="15">
-        <f>G12+H12</f>
+        <f t="shared" si="3"/>
         <v>6.7372800000000002</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>79</v>
-      </c>
       <c r="D13" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="6">
         <v>1.99</v>
@@ -1195,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="6">
-        <f>E13*F13</f>
+        <f t="shared" si="2"/>
         <v>1.99</v>
       </c>
       <c r="H13" s="8">
@@ -1203,22 +1215,22 @@
         <v>0.11144</v>
       </c>
       <c r="I13" s="15">
-        <f>G13+H13</f>
+        <f t="shared" si="3"/>
         <v>2.1014400000000002</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="D14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="6">
         <v>1.91</v>
@@ -1227,29 +1239,29 @@
         <v>1</v>
       </c>
       <c r="G14" s="6">
-        <f>E14*F14</f>
+        <f t="shared" si="2"/>
         <v>1.91</v>
       </c>
       <c r="H14" s="8">
         <v>0</v>
       </c>
       <c r="I14" s="15">
-        <f>G14+H14</f>
+        <f t="shared" si="3"/>
         <v>1.91</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="D15" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="6">
         <v>1.61</v>
@@ -1258,29 +1270,29 @@
         <v>1</v>
       </c>
       <c r="G15" s="6">
-        <f>E15*F15</f>
+        <f t="shared" si="2"/>
         <v>1.61</v>
       </c>
       <c r="H15" s="8">
         <v>0</v>
       </c>
       <c r="I15" s="15">
-        <f>G15+H15</f>
+        <f t="shared" si="3"/>
         <v>1.61</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="E16" s="6">
         <v>0.63</v>
@@ -1289,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="6">
-        <f>E16*F16</f>
+        <f t="shared" si="2"/>
         <v>0.63</v>
       </c>
       <c r="H16" s="8">
@@ -1297,22 +1309,22 @@
         <v>3.5279999999999999E-2</v>
       </c>
       <c r="I16" s="15">
-        <f>G16+H16</f>
+        <f t="shared" si="3"/>
         <v>0.66527999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="E17" s="6">
         <v>0.43</v>
@@ -1321,29 +1333,29 @@
         <v>1</v>
       </c>
       <c r="G17" s="6">
-        <f>E17*F17</f>
+        <f t="shared" si="2"/>
         <v>0.43</v>
       </c>
       <c r="H17" s="8">
         <v>0</v>
       </c>
       <c r="I17" s="15">
-        <f>G17+H17</f>
+        <f t="shared" si="3"/>
         <v>0.43</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="6">
         <v>0.34</v>
@@ -1352,105 +1364,137 @@
         <v>1</v>
       </c>
       <c r="G18" s="6">
-        <f>E18*F18</f>
+        <f t="shared" si="2"/>
         <v>0.34</v>
       </c>
       <c r="H18" s="8">
         <v>0</v>
       </c>
       <c r="I18" s="15">
-        <f>G18+H18</f>
+        <f t="shared" si="3"/>
         <v>0.34</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E19" s="6">
-        <v>0.22</v>
+        <v>0.85</v>
       </c>
       <c r="F19" s="3">
         <v>1</v>
       </c>
       <c r="G19" s="6">
-        <f>E19*F19</f>
-        <v>0.22</v>
+        <f t="shared" ref="G19" si="4">E19*F19</f>
+        <v>0.85</v>
       </c>
       <c r="H19" s="8">
         <f>0.056*G19</f>
-        <v>1.2320000000000001E-2</v>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="I19" s="15">
-        <f>G19+H19</f>
-        <v>0.23232</v>
+        <f t="shared" ref="I19" si="5">G19+H19</f>
+        <v>0.89759999999999995</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="F20" s="3">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6">
+        <f t="shared" si="2"/>
+        <v>0.22</v>
+      </c>
+      <c r="H20" s="8">
+        <f>0.056*G20</f>
+        <v>1.2320000000000001E-2</v>
+      </c>
+      <c r="I20" s="15">
+        <f t="shared" si="3"/>
+        <v>0.23232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="20">
-        <v>1</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="I21" s="22" t="s">
-        <v>69</v>
+      <c r="E22" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="20">
+        <v>1</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1471,12 +1515,14 @@
     <hyperlink ref="D18" r:id="rId11"/>
     <hyperlink ref="D17" r:id="rId12"/>
     <hyperlink ref="D15" r:id="rId13"/>
-    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId14"/>
     <hyperlink ref="D10" r:id="rId15"/>
     <hyperlink ref="D8" r:id="rId16"/>
-    <hyperlink ref="D21" r:id="rId17"/>
+    <hyperlink ref="D22" r:id="rId17"/>
     <hyperlink ref="D9" r:id="rId18"/>
     <hyperlink ref="D13" r:id="rId19"/>
+    <hyperlink ref="C3" r:id="rId20" display="LXFTVP"/>
+    <hyperlink ref="D19" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First Working Gain Scheduled Control
</commit_message>
<xml_diff>
--- a/documentation/microturbineManifast20160930.xlsx
+++ b/documentation/microturbineManifast20160930.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>https://www.amazon.com/ADVANTUS-Polypropylene-Pencil-Inches-34104/dp/B0014DZE8K/ref=sr_1_2?s=office-products&amp;ie=UTF8&amp;qid=1476697766&amp;sr=1-2&amp;keywords=plastic+pencil+box</t>
+  </si>
+  <si>
+    <t>http://www.jameco.com/z/SS-12E17-3-Pin-SPDT-Slide-Switch_2258831.html</t>
   </si>
 </sst>
 </file>
@@ -467,38 +470,39 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="37" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -561,7 +565,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,7 +600,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -807,689 +811,707 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
-    <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31" style="23" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="11" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="15">
         <f>SUM(I2:I23)</f>
-        <v>196.83112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+        <v>199.45112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>20.260000000000002</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>2</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <f t="shared" ref="G2:G9" si="0">E2*F2</f>
         <v>40.520000000000003</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>I2-G2</f>
         <v>8.43</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="7">
         <v>48.95</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>18.89</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
         <f t="shared" si="0"/>
         <v>18.89</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>6.96</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="9">
         <f t="shared" ref="I3:I9" si="1">G3+H3</f>
         <v>25.85</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>18.59</v>
       </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
         <f t="shared" si="0"/>
         <v>18.59</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="10">
         <v>0</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="9">
         <f t="shared" si="1"/>
         <v>18.59</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>17.989999999999998</v>
       </c>
-      <c r="F5" s="3">
-        <v>1</v>
-      </c>
-      <c r="G5" s="6">
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>17.989999999999998</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="10">
         <v>0</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="9">
         <f t="shared" si="1"/>
         <v>17.989999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>16.86</v>
       </c>
-      <c r="F6" s="3">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>16.86</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="10">
         <v>0</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="9">
         <f t="shared" si="1"/>
         <v>16.86</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>4.99</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>9.98</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="10">
         <f>0.056*G7</f>
         <v>0.55888000000000004</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="9">
         <f t="shared" si="1"/>
         <v>10.538880000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>9.9700000000000006</v>
       </c>
-      <c r="F8" s="3">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>9.9700000000000006</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="10">
         <f>0.056*G8</f>
         <v>0.55832000000000004</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="9">
         <f t="shared" si="1"/>
         <v>10.528320000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>17331512</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>8.9700000000000006</v>
       </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="6">
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>8.9700000000000006</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="10">
         <f>0.056*G9</f>
         <v>0.5023200000000001</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="9">
         <f t="shared" si="1"/>
         <v>9.4723199999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>0</v>
       </c>
-      <c r="F10" s="3">
-        <v>1</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
         <v>0</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="10">
         <v>8</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="7">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>6.89</v>
       </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="G11" s="6">
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" ref="G11:G21" si="2">E11*F11</f>
         <v>6.89</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="10">
         <v>0</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="9">
         <f t="shared" ref="I11:I21" si="3">G11+H11</f>
         <v>6.89</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>531137</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>6.38</v>
       </c>
-      <c r="F12" s="3">
-        <v>1</v>
-      </c>
-      <c r="G12" s="6">
+      <c r="F12" s="8">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="2"/>
         <v>6.38</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="10">
         <f>0.056*G12</f>
         <v>0.35727999999999999</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="9">
         <f t="shared" si="3"/>
         <v>6.7372800000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>4.58</v>
       </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="6">
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="2"/>
         <v>4.58</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="10">
         <f>0.056*G13</f>
         <v>0.25647999999999999</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="9">
         <f t="shared" si="3"/>
         <v>4.8364799999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>3.95</v>
       </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" ref="G14" si="4">E14*F14</f>
         <v>3.95</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="10">
         <f>0.056*G14</f>
         <v>0.22120000000000001</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="9">
         <f t="shared" ref="I14" si="5">G14+H14</f>
         <v>4.1711999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>1.99</v>
       </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="6">
+      <c r="F15" s="8">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="2"/>
         <v>1.99</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="10">
         <f>0.056*G15</f>
         <v>0.11144</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="9">
         <f t="shared" si="3"/>
         <v>2.1014400000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>1.91</v>
       </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="5">
         <f t="shared" si="2"/>
         <v>1.91</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="10">
         <v>0</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="9">
         <f t="shared" si="3"/>
         <v>1.91</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="17" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>1.61</v>
       </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="6">
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
         <f t="shared" si="2"/>
         <v>1.61</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="10">
         <v>0</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="9">
         <f t="shared" si="3"/>
         <v>1.61</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>0.63</v>
       </c>
-      <c r="F18" s="3">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6">
+      <c r="F18" s="8">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5">
         <f t="shared" si="2"/>
         <v>0.63</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="10">
         <f>0.056*G18</f>
         <v>3.5279999999999999E-2</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="9">
         <f t="shared" si="3"/>
         <v>0.66527999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="5">
+        <f>2.94/6</f>
+        <v>0.49</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+      <c r="H19" s="5">
+        <f>(3.52+5)/4</f>
+        <v>2.13</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="shared" si="3"/>
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>0.85</v>
       </c>
-      <c r="F20" s="3">
-        <v>1</v>
-      </c>
-      <c r="G20" s="6">
+      <c r="F20" s="8">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
         <f t="shared" ref="G20" si="6">E20*F20</f>
         <v>0.85</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="10">
         <f>0.056*G20</f>
         <v>4.7599999999999996E-2</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="9">
         <f t="shared" ref="I20" si="7">G20+H20</f>
         <v>0.89759999999999995</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="21" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>0.22</v>
       </c>
-      <c r="F21" s="3">
-        <v>1</v>
-      </c>
-      <c r="G21" s="6">
+      <c r="F21" s="8">
+        <v>1</v>
+      </c>
+      <c r="G21" s="5">
         <f t="shared" si="2"/>
         <v>0.22</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="10">
         <f>0.056*G21</f>
         <v>1.2320000000000001E-2</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="9">
         <f t="shared" si="3"/>
         <v>0.23232</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="22" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="F22" s="8">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+    <row r="23" spans="1:9" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1542,8 +1564,9 @@
     <hyperlink ref="D20" r:id="rId18"/>
     <hyperlink ref="D13" r:id="rId19"/>
     <hyperlink ref="D14" r:id="rId20"/>
+    <hyperlink ref="D19" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>